<commit_message>
modificato messaggio conferma salvataggio
</commit_message>
<xml_diff>
--- a/Off_White/Shopify.xlsx
+++ b/Off_White/Shopify.xlsx
@@ -10,7 +10,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="274" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="338" xml:space="preserve">
   <si>
     <t>ID</t>
   </si>
@@ -84,63 +84,13 @@
     <t>Inventory Available: +39 05649689443</t>
   </si>
   <si>
-    <t>8523691262282</t>
-  </si>
-  <si>
-    <t>off-white-artemisia-sunglasses-white</t>
+    <t>8523691327818</t>
+  </si>
+  <si>
+    <t>off-white-arthur-sunglasses-havana</t>
   </si>
   <si>
     <t>MERGE</t>
-  </si>
-  <si>
-    <t>Off White Artemisia White</t>
-  </si>
-  <si>
-    <t>&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Elevate your style with &lt;strong&gt;Off-White sunglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
-&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;This unique &lt;strong&gt;white&lt;/strong&gt; model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the &lt;strong&gt;Off-White Artemisia&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
-&lt;p class="p2" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Discover the latest &lt;a href="/collections/off-white-sunglasses" title="LookerOnline | Off White sunglasses" target="_blank"&gt;Off-White sunglasses 2024 collection&lt;/a&gt; and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Off White</t>
-  </si>
-  <si>
-    <t>Sunglasses</t>
-  </si>
-  <si>
-    <t>10207, Artemisia, Offwhite, spinimages=2, Sunglasses, Unisex, White</t>
-  </si>
-  <si>
-    <t>REPLACE</t>
-  </si>
-  <si>
-    <t>2023-09-26 17:40:34 +0200</t>
-  </si>
-  <si>
-    <t>2023-09-28 12:32:38 +0200</t>
-  </si>
-  <si>
-    <t>Active</t>
-  </si>
-  <si>
-    <t>2023-09-27 11:59:47 +0200</t>
-  </si>
-  <si>
-    <t>https://lookeronline.com/products/off-white-artemisia-sunglasses-white</t>
-  </si>
-  <si>
-    <t>47138254651722</t>
-  </si>
-  <si>
-    <t>ARTEMISIA 10207</t>
-  </si>
-  <si>
-    <t>8052865854535</t>
-  </si>
-  <si>
-    <t>8523691327818</t>
-  </si>
-  <si>
-    <t>off-white-arthur-sunglasses-havana</t>
   </si>
   <si>
     <t>Off White Arthur Havana</t>
@@ -151,13 +101,28 @@
 &lt;p class="p2" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Discover the latest &lt;a href="/collections/off-white-sunglasses" title="LookerOnline | Off White sunglasses" target="_blank"&gt;Off-White sunglasses 2024&lt;/a&gt; collection and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
+    <t>Off White</t>
+  </si>
+  <si>
+    <t>Sunglasses</t>
+  </si>
+  <si>
     <t>26455, Arthur, Havana, Offwhite, spinimages=5, Sunglasses, Unisex</t>
   </si>
   <si>
+    <t>REPLACE</t>
+  </si>
+  <si>
     <t>2023-09-26 17:40:37 +0200</t>
   </si>
   <si>
     <t>2023-09-28 11:54:17 +0200</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>2023-09-27 11:59:47 +0200</t>
   </si>
   <si>
     <t>https://lookeronline.com/products/off-white-arthur-sunglasses-havana</t>
@@ -190,6 +155,9 @@
   </si>
   <si>
     <t>2023-09-26 17:40:39 +0200</t>
+  </si>
+  <si>
+    <t>2023-09-28 12:32:38 +0200</t>
   </si>
   <si>
     <t>https://lookeronline.com/products/off-white-arthur-sunglasses-black</t>
@@ -237,6 +205,107 @@
     <t>8051594080369</t>
   </si>
   <si>
+    <t>8523691262282</t>
+  </si>
+  <si>
+    <t>off-white-artemisia-sunglasses-white</t>
+  </si>
+  <si>
+    <t>Off White Artemisia White</t>
+  </si>
+  <si>
+    <t>&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Elevate your style with &lt;strong&gt;Off-White sunglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
+&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;This unique &lt;strong&gt;white&lt;/strong&gt; model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the &lt;strong&gt;Off-White Artemisia&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
+&lt;p class="p2" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Discover the latest &lt;a href="/collections/off-white-sunglasses" title="LookerOnline | Off White sunglasses" target="_blank"&gt;Off-White sunglasses 2024 collection&lt;/a&gt; and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>10207, Artemisia, Offwhite, spinimages=2, Sunglasses, Unisex, White</t>
+  </si>
+  <si>
+    <t>2023-09-26 17:40:34 +0200</t>
+  </si>
+  <si>
+    <t>https://lookeronline.com/products/off-white-artemisia-sunglasses-white</t>
+  </si>
+  <si>
+    <t>47138254651722</t>
+  </si>
+  <si>
+    <t>ARTEMISIA 10207</t>
+  </si>
+  <si>
+    <t>8052865854535</t>
+  </si>
+  <si>
+    <t>8523691491658</t>
+  </si>
+  <si>
+    <t>off-white-cady-sunglasses-black</t>
+  </si>
+  <si>
+    <t>Off White Cady Black</t>
+  </si>
+  <si>
+    <t>&lt;meta charset="utf-8"&gt;
+&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Elevate your style with&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White sunglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
+&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;This unique &lt;strong data-mce-fragment="1"&gt;black&lt;/strong&gt; model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Cady&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
+&lt;p class="p2" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Discover the latest&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;a href="https://admin.shopify.com/collections/off-white-sunglasses" title="LookerOnline | Off White sunglasses" data-mce-fragment="1" data-mce-href="https://admin.shopify.com/collections/off-white-sunglasses" target="_blank"&gt;Off-White sunglasses 2024&lt;/a&gt; collection and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>11007, Black, Cady, Offwhite, spinimages=5, Sunglasses, Unisex</t>
+  </si>
+  <si>
+    <t>2023-09-26 17:40:44 +0200</t>
+  </si>
+  <si>
+    <t>2023-09-27 11:59:48 +0200</t>
+  </si>
+  <si>
+    <t>https://lookeronline.com/products/off-white-cady-sunglasses-black</t>
+  </si>
+  <si>
+    <t>47138254979402</t>
+  </si>
+  <si>
+    <t>CADY 11007</t>
+  </si>
+  <si>
+    <t>8052865781251</t>
+  </si>
+  <si>
+    <t>8523691589962</t>
+  </si>
+  <si>
+    <t>off-white-catalina-sunglasses-black</t>
+  </si>
+  <si>
+    <t>Off White Catalina Black</t>
+  </si>
+  <si>
+    <t>&lt;meta charset="utf-8"&gt;
+&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Elevate your style with&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White sunglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
+&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;This unique &lt;strong data-mce-fragment="1"&gt;black&lt;/strong&gt; model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Catalina&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
+&lt;p class="p2" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Discover the latest&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;a href="https://admin.shopify.com/collections/off-white-sunglasses" title="LookerOnline | Off White sunglasses" data-mce-fragment="1" data-mce-href="https://admin.shopify.com/collections/off-white-sunglasses" target="_blank"&gt;Off-White sunglasses 2024&lt;/a&gt; collection and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>11007, Black, Catalina, Dark, Grey, Offwhite, spinimages=5, Sunglasses, Unisex</t>
+  </si>
+  <si>
+    <t>2023-09-26 17:40:49 +0200</t>
+  </si>
+  <si>
+    <t>https://lookeronline.com/products/off-white-catalina-sunglasses-black</t>
+  </si>
+  <si>
+    <t>47138256879946</t>
+  </si>
+  <si>
+    <t>CATALINA 11007</t>
+  </si>
+  <si>
+    <t>8052865781268</t>
+  </si>
+  <si>
     <t>8523691557194</t>
   </si>
   <si>
@@ -261,9 +330,6 @@
     <t>2023-09-28 11:54:18 +0200</t>
   </si>
   <si>
-    <t>2023-09-27 11:59:48 +0200</t>
-  </si>
-  <si>
     <t>https://lookeronline.com/products/off-white-catalina-sunglasses-fuchsia</t>
   </si>
   <si>
@@ -274,39 +340,6 @@
   </si>
   <si>
     <t>8051594080055</t>
-  </si>
-  <si>
-    <t>8523691491658</t>
-  </si>
-  <si>
-    <t>off-white-cady-sunglasses-black</t>
-  </si>
-  <si>
-    <t>Off White Cady Black</t>
-  </si>
-  <si>
-    <t>&lt;meta charset="utf-8"&gt;
-&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Elevate your style with&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White sunglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
-&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;This unique &lt;strong data-mce-fragment="1"&gt;black&lt;/strong&gt; model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Cady&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
-&lt;p class="p2" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Discover the latest&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;a href="https://admin.shopify.com/collections/off-white-sunglasses" title="LookerOnline | Off White sunglasses" data-mce-fragment="1" data-mce-href="https://admin.shopify.com/collections/off-white-sunglasses" target="_blank"&gt;Off-White sunglasses 2024&lt;/a&gt; collection and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>11007, Black, Cady, Offwhite, spinimages=5, Sunglasses, Unisex</t>
-  </si>
-  <si>
-    <t>2023-09-26 17:40:44 +0200</t>
-  </si>
-  <si>
-    <t>https://lookeronline.com/products/off-white-cady-sunglasses-black</t>
-  </si>
-  <si>
-    <t>47138254979402</t>
-  </si>
-  <si>
-    <t>CADY 11007</t>
-  </si>
-  <si>
-    <t>8052865781251</t>
   </si>
   <si>
     <t>8523691622730</t>
@@ -342,37 +375,43 @@
     <t>8052865854290</t>
   </si>
   <si>
-    <t>8523691589962</t>
-  </si>
-  <si>
-    <t>off-white-catalina-sunglasses-black</t>
-  </si>
-  <si>
-    <t>Off White Catalina Black</t>
+    <t>8523691786570</t>
+  </si>
+  <si>
+    <t>off-white-leonardo-sunglasses-white</t>
+  </si>
+  <si>
+    <t>Off White Leonardo White</t>
   </si>
   <si>
     <t>&lt;meta charset="utf-8"&gt;
 &lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Elevate your style with&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White sunglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
-&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;This unique &lt;strong data-mce-fragment="1"&gt;black&lt;/strong&gt; model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Catalina&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
+&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;This unique &lt;strong data-mce-fragment="1"&gt;white&lt;/strong&gt; model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Leonardo&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
 &lt;p class="p2" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Discover the latest&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;a href="https://admin.shopify.com/collections/off-white-sunglasses" title="LookerOnline | Off White sunglasses" data-mce-fragment="1" data-mce-href="https://admin.shopify.com/collections/off-white-sunglasses" target="_blank"&gt;Off-White sunglasses 2024&lt;/a&gt; collection and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>11007, Black, Catalina, Dark, Grey, Offwhite, spinimages=5, Sunglasses, Unisex</t>
-  </si>
-  <si>
-    <t>2023-09-26 17:40:49 +0200</t>
-  </si>
-  <si>
-    <t>https://lookeronline.com/products/off-white-catalina-sunglasses-black</t>
-  </si>
-  <si>
-    <t>47138256879946</t>
-  </si>
-  <si>
-    <t>CATALINA 11007</t>
-  </si>
-  <si>
-    <t>8052865781268</t>
+    <t>10107, Leonardo, Offwhite, spinimages=3, Sunglasses, Unisex, White</t>
+  </si>
+  <si>
+    <t>2023-09-26 17:40:57 +0200</t>
+  </si>
+  <si>
+    <t>2023-09-28 11:54:19 +0200</t>
+  </si>
+  <si>
+    <t>2023-09-27 11:59:49 +0200</t>
+  </si>
+  <si>
+    <t>https://lookeronline.com/products/off-white-leonardo-sunglasses-white</t>
+  </si>
+  <si>
+    <t>47138257011018</t>
+  </si>
+  <si>
+    <t>LEONARDO 10107</t>
+  </si>
+  <si>
+    <t>8051594080062</t>
   </si>
   <si>
     <t>8523691688266</t>
@@ -399,9 +438,6 @@
     <t>2023-09-28 12:32:39 +0200</t>
   </si>
   <si>
-    <t>2023-09-27 11:59:49 +0200</t>
-  </si>
-  <si>
     <t>https://lookeronline.com/products/off-white-francisco-sunglasses-blue</t>
   </si>
   <si>
@@ -412,42 +448,6 @@
   </si>
   <si>
     <t>8052865854313</t>
-  </si>
-  <si>
-    <t>8523691786570</t>
-  </si>
-  <si>
-    <t>off-white-leonardo-sunglasses-white</t>
-  </si>
-  <si>
-    <t>Off White Leonardo White</t>
-  </si>
-  <si>
-    <t>&lt;meta charset="utf-8"&gt;
-&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Elevate your style with&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White sunglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
-&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;This unique &lt;strong data-mce-fragment="1"&gt;white&lt;/strong&gt; model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Leonardo&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
-&lt;p class="p2" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Discover the latest&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;a href="https://admin.shopify.com/collections/off-white-sunglasses" title="LookerOnline | Off White sunglasses" data-mce-fragment="1" data-mce-href="https://admin.shopify.com/collections/off-white-sunglasses" target="_blank"&gt;Off-White sunglasses 2024&lt;/a&gt; collection and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>10107, Leonardo, Offwhite, spinimages=3, Sunglasses, Unisex, White</t>
-  </si>
-  <si>
-    <t>2023-09-26 17:40:57 +0200</t>
-  </si>
-  <si>
-    <t>2023-09-28 11:54:19 +0200</t>
-  </si>
-  <si>
-    <t>https://lookeronline.com/products/off-white-leonardo-sunglasses-white</t>
-  </si>
-  <si>
-    <t>47138257011018</t>
-  </si>
-  <si>
-    <t>LEONARDO 10107</t>
-  </si>
-  <si>
-    <t>8051594080062</t>
   </si>
   <si>
     <t>8523691884874</t>
@@ -516,6 +516,42 @@
     <t>8051594080079</t>
   </si>
   <si>
+    <t>8523692409162</t>
+  </si>
+  <si>
+    <t>off-white-savannah-sunglasses-havana</t>
+  </si>
+  <si>
+    <t>Off White Savannah Havana</t>
+  </si>
+  <si>
+    <t>&lt;meta charset="utf-8"&gt;
+&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Elevate your style with&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White sunglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
+&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;This unique &lt;strong data-mce-fragment="1"&gt;havana &lt;/strong&gt;model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Savannah&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
+&lt;p class="p2" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Discover the latest&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;a href="https://admin.shopify.com/collections/off-white-sunglasses" title="LookerOnline | Off White sunglasses" data-mce-fragment="1" data-mce-href="https://admin.shopify.com/collections/off-white-sunglasses" target="_blank"&gt;Off-White sunglasses 2024&lt;/a&gt; collection and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>16055, Havana, Offwhite, Savannah, spinimages=5, Sunglasses, Unisex</t>
+  </si>
+  <si>
+    <t>2023-09-26 17:41:22 +0200</t>
+  </si>
+  <si>
+    <t>2023-09-27 11:59:52 +0200</t>
+  </si>
+  <si>
+    <t>https://lookeronline.com/products/off-white-savannah-sunglasses-havana</t>
+  </si>
+  <si>
+    <t>47138259894602</t>
+  </si>
+  <si>
+    <t>SAVANNAH 16055</t>
+  </si>
+  <si>
+    <t>8051594079806</t>
+  </si>
+  <si>
     <t>8523692048714</t>
   </si>
   <si>
@@ -552,42 +588,6 @@
     <t>8052865854405</t>
   </si>
   <si>
-    <t>8523692409162</t>
-  </si>
-  <si>
-    <t>off-white-savannah-sunglasses-havana</t>
-  </si>
-  <si>
-    <t>Off White Savannah Havana</t>
-  </si>
-  <si>
-    <t>&lt;meta charset="utf-8"&gt;
-&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Elevate your style with&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White sunglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
-&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;This unique &lt;strong data-mce-fragment="1"&gt;havana &lt;/strong&gt;model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Savannah&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
-&lt;p class="p2" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Discover the latest&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;a href="https://admin.shopify.com/collections/off-white-sunglasses" title="LookerOnline | Off White sunglasses" data-mce-fragment="1" data-mce-href="https://admin.shopify.com/collections/off-white-sunglasses" target="_blank"&gt;Off-White sunglasses 2024&lt;/a&gt; collection and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>16055, Havana, Offwhite, Savannah, spinimages=5, Sunglasses, Unisex</t>
-  </si>
-  <si>
-    <t>2023-09-26 17:41:22 +0200</t>
-  </si>
-  <si>
-    <t>2023-09-27 11:59:52 +0200</t>
-  </si>
-  <si>
-    <t>https://lookeronline.com/products/off-white-savannah-sunglasses-havana</t>
-  </si>
-  <si>
-    <t>47138259894602</t>
-  </si>
-  <si>
-    <t>SAVANNAH 16055</t>
-  </si>
-  <si>
-    <t>8051594079806</t>
-  </si>
-  <si>
     <t>8523692540234</t>
   </si>
   <si>
@@ -663,6 +663,42 @@
     <t>8051594080215</t>
   </si>
   <si>
+    <t>8523692638538</t>
+  </si>
+  <si>
+    <t>off-white-virgil-sunglasses-dark-grey</t>
+  </si>
+  <si>
+    <t>Off White Virgil Black</t>
+  </si>
+  <si>
+    <t>&lt;meta charset="utf-8"&gt;
+&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Elevate your style with&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White sunglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
+&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;This unique &lt;strong&gt;black &lt;/strong&gt;model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Virgil&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
+&lt;p class="p2" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Discover the latest&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;a href="https://admin.shopify.com/collections/off-white-sunglasses" title="LookerOnline | Off White sunglasses" data-mce-fragment="1" data-mce-href="https://admin.shopify.com/collections/off-white-sunglasses" target="_blank"&gt;Off-White sunglasses 2024&lt;/a&gt; collection and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>11007, Black, Dark, Grey, Offwhite, spinimages=5, Sunglasses, Unisex, Virgil</t>
+  </si>
+  <si>
+    <t>2023-09-26 17:41:32 +0200</t>
+  </si>
+  <si>
+    <t>2023-09-28 11:54:20 +0200</t>
+  </si>
+  <si>
+    <t>https://lookeronline.com/products/off-white-virgil-sunglasses-dark-grey</t>
+  </si>
+  <si>
+    <t>47138260123978</t>
+  </si>
+  <si>
+    <t>VIRGIL 11007</t>
+  </si>
+  <si>
+    <t>8052865781282</t>
+  </si>
+  <si>
     <t>8523692605770</t>
   </si>
   <si>
@@ -699,40 +735,73 @@
     <t>8052865804356</t>
   </si>
   <si>
-    <t>8523692638538</t>
-  </si>
-  <si>
-    <t>off-white-virgil-sunglasses-dark-grey</t>
-  </si>
-  <si>
-    <t>Off White Virgil Black</t>
+    <t>8523692671306</t>
+  </si>
+  <si>
+    <t>off-white-virgil-sunglasses-havana</t>
+  </si>
+  <si>
+    <t>Off White Virgil Havana</t>
   </si>
   <si>
     <t>&lt;meta charset="utf-8"&gt;
 &lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Elevate your style with&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White sunglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
-&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;This unique &lt;strong&gt;black &lt;/strong&gt;model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Virgil&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
+&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;This unique &lt;strong&gt;havana &lt;/strong&gt;model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Virgil&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
 &lt;p class="p2" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Discover the latest&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;a href="https://admin.shopify.com/collections/off-white-sunglasses" title="LookerOnline | Off White sunglasses" data-mce-fragment="1" data-mce-href="https://admin.shopify.com/collections/off-white-sunglasses" target="_blank"&gt;Off-White sunglasses 2024&lt;/a&gt; collection and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>11007, Black, Dark, Grey, Offwhite, spinimages=5, Sunglasses, Unisex, Virgil</t>
-  </si>
-  <si>
-    <t>2023-09-26 17:41:32 +0200</t>
-  </si>
-  <si>
-    <t>2023-09-28 11:54:20 +0200</t>
-  </si>
-  <si>
-    <t>https://lookeronline.com/products/off-white-virgil-sunglasses-dark-grey</t>
-  </si>
-  <si>
-    <t>47138260123978</t>
-  </si>
-  <si>
-    <t>VIRGIL 11007</t>
-  </si>
-  <si>
-    <t>8052865781282</t>
+    <t>26455, Havana, Offwhite, spinimages=5, Sunglasses, Unisex, Virgil</t>
+  </si>
+  <si>
+    <t>2023-09-26 17:41:35 +0200</t>
+  </si>
+  <si>
+    <t>2023-09-27 11:59:54 +0200</t>
+  </si>
+  <si>
+    <t>https://lookeronline.com/products/off-white-virgil-sunglasses-havana</t>
+  </si>
+  <si>
+    <t>47138260189514</t>
+  </si>
+  <si>
+    <t>VIRGIL 26455</t>
+  </si>
+  <si>
+    <t>8052865804363</t>
+  </si>
+  <si>
+    <t>8523692769610</t>
+  </si>
+  <si>
+    <t>off-white-volcanite-sunglasses-black</t>
+  </si>
+  <si>
+    <t>Off White Volcanite Black</t>
+  </si>
+  <si>
+    <t>&lt;meta charset="utf-8"&gt;
+&lt;p data-mce-fragment="1" class="p1"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;Elevate your style with&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White sunglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
+&lt;p data-mce-fragment="1" class="p1"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;This unique &lt;strong data-mce-fragment="1"&gt;black &lt;/strong&gt;model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Volcanite&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
+&lt;p data-mce-fragment="1" class="p2"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;Discover the latest&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;a data-mce-fragment="1" title="LookerOnline | Off White sunglasses" href="https://admin.shopify.com/collections/off-white-sunglasses" target="_blank" data-mce-href="https://admin.shopify.com/collections/off-white-sunglasses"&gt;Off-White sunglasses 2024&lt;/a&gt; collection and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>11007, Black, Offwhite, spinimages=4, Sunglasses, Unisex, Volcanite</t>
+  </si>
+  <si>
+    <t>2023-09-26 17:41:37 +0200</t>
+  </si>
+  <si>
+    <t>https://lookeronline.com/products/off-white-volcanite-sunglasses-black</t>
+  </si>
+  <si>
+    <t>47138260255050</t>
+  </si>
+  <si>
+    <t>VOLCANITE 11007</t>
+  </si>
+  <si>
+    <t>8051594376875</t>
   </si>
   <si>
     <t>8523692802378</t>
@@ -756,9 +825,6 @@
     <t>2023-09-26 17:41:40 +0200</t>
   </si>
   <si>
-    <t>2023-09-27 11:59:54 +0200</t>
-  </si>
-  <si>
     <t>https://lookeronline.com/products/off-white-zurich-sunglasses-black</t>
   </si>
   <si>
@@ -771,70 +837,214 @@
     <t>8051594030036</t>
   </si>
   <si>
-    <t>8523692671306</t>
-  </si>
-  <si>
-    <t>off-white-virgil-sunglasses-havana</t>
-  </si>
-  <si>
-    <t>Off White Virgil Havana</t>
+    <t>8523692179786</t>
+  </si>
+  <si>
+    <t>off-white-style-28-eyeglasses-havana</t>
+  </si>
+  <si>
+    <t>Optical Style 28 Havana</t>
   </si>
   <si>
     <t>&lt;meta charset="utf-8"&gt;
-&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Elevate your style with&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White sunglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
-&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;This unique &lt;strong&gt;havana &lt;/strong&gt;model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Virgil&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
+&lt;p data-mce-fragment="1" class="p1"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;Elevate your style with&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White eyeglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
+&lt;p data-mce-fragment="1" class="p1"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;This unique &lt;strong data-mce-fragment="1"&gt;havana &lt;/strong&gt;model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Optical Style 28&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
+&lt;p data-mce-fragment="1" class="p2"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;Discover the latest&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;a data-mce-fragment="1" title="LookerOnline | Off White sunglasses" href="https://admin.shopify.com/collections/off-white-sunglasses" target="_blank" data-mce-href="https://admin.shopify.com/collections/off-white-sunglasses"&gt;Off-White sunglasses 2024&lt;/a&gt; collection and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Eyeglasses</t>
+  </si>
+  <si>
+    <t>16000, Eyeglasses, Havana, Offwhite, Style28, Unisex</t>
+  </si>
+  <si>
+    <t>2023-09-26 17:41:12 +0200</t>
+  </si>
+  <si>
+    <t>2023-09-28 12:32:41 +0200</t>
+  </si>
+  <si>
+    <t>https://lookeronline.com/products/off-white-style-28-eyeglasses-havana</t>
+  </si>
+  <si>
+    <t>47138258977098</t>
+  </si>
+  <si>
+    <t>STYLE 28 16000</t>
+  </si>
+  <si>
+    <t>8051594080543</t>
+  </si>
+  <si>
+    <t>8523692114250</t>
+  </si>
+  <si>
+    <t>off-white-style-21-eyeglasses-havana</t>
+  </si>
+  <si>
+    <t>Optical Style 21 Havana</t>
+  </si>
+  <si>
+    <t>&lt;meta charset="utf-8"&gt;
+&lt;p data-mce-fragment="1" class="p1"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;Elevate your style with&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White eyeglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
+&lt;p data-mce-fragment="1" class="p1"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;This unique &lt;strong&gt;havana &lt;/strong&gt;model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Optical Style 21&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
+&lt;p data-mce-fragment="1" class="p2"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;Discover the latest&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;a data-mce-fragment="1" title="LookerOnline | Off White sunglasses" href="https://admin.shopify.com/collections/off-white-sunglasses" target="_blank" data-mce-href="https://admin.shopify.com/collections/off-white-sunglasses"&gt;Off-White sunglasses 2024&lt;/a&gt; collection and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>16000, Eyeglasses, Havana, Offwhite, Style21, Unisex</t>
+  </si>
+  <si>
+    <t>2023-09-26 17:41:10 +0200</t>
+  </si>
+  <si>
+    <t>https://lookeronline.com/products/off-white-style-21-eyeglasses-havana</t>
+  </si>
+  <si>
+    <t>47138258911562</t>
+  </si>
+  <si>
+    <t>STYLE 21 16000</t>
+  </si>
+  <si>
+    <t>8051594032214</t>
+  </si>
+  <si>
+    <t>8523692081482</t>
+  </si>
+  <si>
+    <t>off-white-style-21-eyeglasses-black</t>
+  </si>
+  <si>
+    <t>Optical Style 21 Black</t>
+  </si>
+  <si>
+    <t>&lt;meta charset="utf-8"&gt;
+&lt;p data-mce-fragment="1" class="p1"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;Elevate your style with&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White eyeglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
+&lt;p data-mce-fragment="1" class="p1"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;This unique &lt;strong&gt;black &lt;/strong&gt;model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Optical Style 21&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
+&lt;p data-mce-fragment="1" class="p2"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;Discover the latest&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;a data-mce-fragment="1" title="LookerOnline | Off White sunglasses" href="https://admin.shopify.com/collections/off-white-sunglasses" target="_blank" data-mce-href="https://admin.shopify.com/collections/off-white-sunglasses"&gt;Off-White sunglasses 2024&lt;/a&gt; collection and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>11000, Black, Eyeglasses, Offwhite, Style21, Unisex</t>
+  </si>
+  <si>
+    <t>2023-09-26 17:41:07 +0200</t>
+  </si>
+  <si>
+    <t>2023-09-28 11:54:22 +0200</t>
+  </si>
+  <si>
+    <t>https://lookeronline.com/products/off-white-style-21-eyeglasses-black</t>
+  </si>
+  <si>
+    <t>47138258813258</t>
+  </si>
+  <si>
+    <t>STYLE 21 11000</t>
+  </si>
+  <si>
+    <t>8051594032207</t>
+  </si>
+  <si>
+    <t>8523692245322</t>
+  </si>
+  <si>
+    <t>off-white-style-29-eyeglasses-black</t>
+  </si>
+  <si>
+    <t>Optical Style 29 Black</t>
+  </si>
+  <si>
+    <t>&lt;meta charset="utf-8"&gt;
+&lt;p data-mce-fragment="1" class="p1"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;Elevate your style with&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White eyeglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
+&lt;p data-mce-fragment="1" class="p1"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;This unique &lt;strong&gt;black &lt;/strong&gt;model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Optical Style 29&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
+&lt;p data-mce-fragment="1" class="p2"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;Discover the latest&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;a data-mce-fragment="1" title="LookerOnline | Off White sunglasses" href="https://admin.shopify.com/collections/off-white-sunglasses" target="_blank" data-mce-href="https://admin.shopify.com/collections/off-white-sunglasses"&gt;Off-White sunglasses 2024&lt;/a&gt; collection and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Black, Eyeglasses, Offwhite, Style29 11000, Unisex</t>
+  </si>
+  <si>
+    <t>2023-09-26 17:41:15 +0200</t>
+  </si>
+  <si>
+    <t>https://lookeronline.com/products/off-white-style-29-eyeglasses-black</t>
+  </si>
+  <si>
+    <t>47138259272010</t>
+  </si>
+  <si>
+    <t>STYLE 29 11000</t>
+  </si>
+  <si>
+    <t>8051594079998</t>
+  </si>
+  <si>
+    <t>8523692376394</t>
+  </si>
+  <si>
+    <t>off-white-style-29-eyeglasses-white</t>
+  </si>
+  <si>
+    <t>Optical Style 29 White</t>
+  </si>
+  <si>
+    <t>&lt;meta charset="utf-8"&gt;
+&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Elevate your style with&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White eyeglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
+&lt;p class="p1" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;This unique &lt;strong&gt;white &lt;/strong&gt;model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Optical Style 29&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
 &lt;p class="p2" data-mce-fragment="1"&gt;&lt;span class="s1" data-mce-fragment="1"&gt;Discover the latest&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;a href="https://admin.shopify.com/collections/off-white-sunglasses" title="LookerOnline | Off White sunglasses" data-mce-fragment="1" data-mce-href="https://admin.shopify.com/collections/off-white-sunglasses" target="_blank"&gt;Off-White sunglasses 2024&lt;/a&gt; collection and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>26455, Havana, Offwhite, spinimages=5, Sunglasses, Unisex, Virgil</t>
-  </si>
-  <si>
-    <t>2023-09-26 17:41:35 +0200</t>
-  </si>
-  <si>
-    <t>https://lookeronline.com/products/off-white-virgil-sunglasses-havana</t>
-  </si>
-  <si>
-    <t>47138260189514</t>
-  </si>
-  <si>
-    <t>VIRGIL 26455</t>
-  </si>
-  <si>
-    <t>8052865804363</t>
-  </si>
-  <si>
-    <t>8523692769610</t>
-  </si>
-  <si>
-    <t>off-white-volcanite-sunglasses-black</t>
-  </si>
-  <si>
-    <t>Off White Volcanite Black</t>
+    <t>10100, Eyeglasses, Offwhite, Style29, Unisex, White</t>
+  </si>
+  <si>
+    <t>2023-09-26 17:41:20 +0200</t>
+  </si>
+  <si>
+    <t>https://lookeronline.com/products/off-white-style-29-eyeglasses-white</t>
+  </si>
+  <si>
+    <t>47138259829066</t>
+  </si>
+  <si>
+    <t>STYLE 29 10100</t>
+  </si>
+  <si>
+    <t>8051594079974</t>
+  </si>
+  <si>
+    <t>8523692310858</t>
+  </si>
+  <si>
+    <t>off-white-style-29-eyeglasses-havana</t>
+  </si>
+  <si>
+    <t>Optical Style 29 Havana</t>
   </si>
   <si>
     <t>&lt;meta charset="utf-8"&gt;
-&lt;p data-mce-fragment="1" class="p1"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;Elevate your style with&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White sunglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
-&lt;p data-mce-fragment="1" class="p1"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;This unique &lt;strong data-mce-fragment="1"&gt;black &lt;/strong&gt;model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Volcanite&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
+&lt;p data-mce-fragment="1" class="p1"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;Elevate your style with&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White eyeglasses&lt;/strong&gt;, a fashion-forward choice that embodies modern luxury and streetwear aesthetics. Crafted with precision and attention to detail, these shades are designed to make a statement.&lt;/span&gt;&lt;/p&gt;
+&lt;p data-mce-fragment="1" class="p1"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;This unique &lt;strong data-mce-fragment="1"&gt;havana &lt;/strong&gt;model represents Off-White's distinctive approach to eyewear, blending high fashion with urban culture. Created in collaboration with renowned eyewear producers, the&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;strong data-mce-fragment="1"&gt;Off-White&lt;span data-mce-fragment="1"&gt; Optical Style 29&lt;/span&gt;&lt;/strong&gt; exudes sophistication and edge, adding a touch of avant-garde to your look.&lt;/span&gt;&lt;/p&gt;
 &lt;p data-mce-fragment="1" class="p2"&gt;&lt;span data-mce-fragment="1" class="s1"&gt;Discover the latest&lt;span data-mce-fragment="1"&gt; &lt;/span&gt;&lt;a data-mce-fragment="1" title="LookerOnline | Off White sunglasses" href="https://admin.shopify.com/collections/off-white-sunglasses" target="_blank" data-mce-href="https://admin.shopify.com/collections/off-white-sunglasses"&gt;Off-White sunglasses 2024&lt;/a&gt; collection and step into a world where fashion meets art. With these shades, you're not just wearing sunglasses; you're making a bold fashion statement.&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>11007, Black, Offwhite, spinimages=4, Sunglasses, Unisex, Volcanite</t>
-  </si>
-  <si>
-    <t>2023-09-26 17:41:37 +0200</t>
-  </si>
-  <si>
-    <t>https://lookeronline.com/products/off-white-volcanite-sunglasses-black</t>
-  </si>
-  <si>
-    <t>47138260255050</t>
-  </si>
-  <si>
-    <t>VOLCANITE 11007</t>
-  </si>
-  <si>
-    <t>8051594376875</t>
+    <t>Eyeglasses, Havana, Offwhite, Style29 16000, Unisex</t>
+  </si>
+  <si>
+    <t>2023-09-26 17:41:17 +0200</t>
+  </si>
+  <si>
+    <t>2023-09-28 11:54:23 +0200</t>
+  </si>
+  <si>
+    <t>https://lookeronline.com/products/off-white-style-29-eyeglasses-havana</t>
+  </si>
+  <si>
+    <t>47138259632458</t>
+  </si>
+  <si>
+    <t>STYLE 29 16000</t>
+  </si>
+  <si>
+    <t>8051594080000</t>
   </si>
   <si>
     <t>Job ID</t>
@@ -867,22 +1077,22 @@
     <t>Filters</t>
   </si>
   <si>
-    <t>229824889</t>
+    <t>232665649</t>
   </si>
   <si>
     <t>Products</t>
   </si>
   <si>
-    <t>2023-10-17 16:09:10 +0200</t>
-  </si>
-  <si>
-    <t>2023-10-17 16:09:15 +0200</t>
-  </si>
-  <si>
-    <t>00:00:04</t>
-  </si>
-  <si>
-    <t>21 of 38451</t>
+    <t>2023-10-26 14:51:51 +0200</t>
+  </si>
+  <si>
+    <t>2023-10-26 14:51:56 +0200</t>
+  </si>
+  <si>
+    <t>00:00:05</t>
+  </si>
+  <si>
+    <t>27 of 40443</t>
   </si>
   <si>
     <t>Base, Variants, Inventory Levels</t>
@@ -892,7 +1102,7 @@
   </si>
   <si>
     <t>Tags: not equal to any of: Outlet
-Type: equals to any of: Sunglasses
+Type: equals to any of: Sunglasses, Eyeglasses
 Vendor: equals to any of: Off White</t>
   </si>
 </sst>
@@ -1033,7 +1243,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:X22"/>
+  <dimension ref="A1:X28"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0">
       <pane topLeftCell="C2" state="frozenSplit" activePane="bottomRight" ySplit="1" xSplit="2"/>
@@ -1198,10 +1408,10 @@
         <v>40</v>
       </c>
       <c r="T2" s="4" t="n">
-        <v>250.0</v>
+        <v>245.0</v>
       </c>
       <c r="U2" s="4" t="n">
-        <v>250.0</v>
+        <v>245.0</v>
       </c>
       <c r="V2" s="3" t="n">
         <v>1</v>
@@ -1342,10 +1552,10 @@
         <v>61</v>
       </c>
       <c r="T4" s="4" t="n">
-        <v>245.0</v>
+        <v>280.0</v>
       </c>
       <c r="U4" s="4" t="n">
-        <v>245.0</v>
+        <v>280.0</v>
       </c>
       <c r="V4" s="3" t="n">
         <v>1</v>
@@ -1414,10 +1624,10 @@
         <v>71</v>
       </c>
       <c r="T5" s="4" t="n">
-        <v>280.0</v>
+        <v>250.0</v>
       </c>
       <c r="U5" s="4" t="n">
-        <v>280.0</v>
+        <v>250.0</v>
       </c>
       <c r="V5" s="3" t="n">
         <v>1</v>
@@ -1461,7 +1671,7 @@
         <v>77</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="L6" s="0" t="s">
         <v>35</v>
@@ -1470,52 +1680,52 @@
         <v>1</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O6" s="0"/>
       <c r="P6" s="0" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q6" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="Q6" s="0" t="s">
+      <c r="R6" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="R6" s="0" t="s">
+      <c r="S6" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="S6" s="0" t="s">
-        <v>83</v>
-      </c>
       <c r="T6" s="4" t="n">
-        <v>250.0</v>
+        <v>280.0</v>
       </c>
       <c r="U6" s="4" t="n">
-        <v>250.0</v>
+        <v>280.0</v>
       </c>
       <c r="V6" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="X6" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>84</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>85</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>26</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="E7" s="0" t="s">
         <v>86</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>87</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>29</v>
@@ -1524,16 +1734,16 @@
         <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>32</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="L7" s="0" t="s">
         <v>35</v>
@@ -1542,26 +1752,26 @@
         <v>1</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O7" s="0"/>
       <c r="P7" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q7" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="Q7" s="0" t="s">
+      <c r="R7" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="R7" s="0" t="s">
+      <c r="S7" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="S7" s="0" t="s">
-        <v>93</v>
-      </c>
       <c r="T7" s="4" t="n">
-        <v>280.0</v>
+        <v>250.0</v>
       </c>
       <c r="U7" s="4" t="n">
-        <v>280.0</v>
+        <v>250.0</v>
       </c>
       <c r="V7" s="3" t="n">
         <v>2</v>
@@ -1575,19 +1785,19 @@
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>95</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>26</v>
       </c>
       <c r="D8" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>97</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>29</v>
@@ -1596,16 +1806,16 @@
         <v>30</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>32</v>
       </c>
       <c r="J8" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="K8" s="0" t="s">
         <v>99</v>
-      </c>
-      <c r="K8" s="0" t="s">
-        <v>78</v>
       </c>
       <c r="L8" s="0" t="s">
         <v>35</v>
@@ -1614,7 +1824,7 @@
         <v>1</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O8" s="0"/>
       <c r="P8" s="0" t="s">
@@ -1630,10 +1840,10 @@
         <v>103</v>
       </c>
       <c r="T8" s="4" t="n">
-        <v>275.0</v>
+        <v>250.0</v>
       </c>
       <c r="U8" s="4" t="n">
-        <v>275.0</v>
+        <v>250.0</v>
       </c>
       <c r="V8" s="3" t="n">
         <v>1</v>
@@ -1677,7 +1887,7 @@
         <v>109</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>34</v>
+        <v>99</v>
       </c>
       <c r="L9" s="0" t="s">
         <v>35</v>
@@ -1686,7 +1896,7 @@
         <v>1</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O9" s="0"/>
       <c r="P9" s="0" t="s">
@@ -1702,19 +1912,19 @@
         <v>113</v>
       </c>
       <c r="T9" s="4" t="n">
-        <v>250.0</v>
+        <v>275.0</v>
       </c>
       <c r="U9" s="4" t="n">
-        <v>250.0</v>
+        <v>275.0</v>
       </c>
       <c r="V9" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W9" s="3" t="n">
         <v>0</v>
       </c>
       <c r="X9" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -1774,10 +1984,10 @@
         <v>125</v>
       </c>
       <c r="T10" s="4" t="n">
-        <v>275.0</v>
+        <v>350.0</v>
       </c>
       <c r="U10" s="4" t="n">
-        <v>275.0</v>
+        <v>350.0</v>
       </c>
       <c r="V10" s="3" t="n">
         <v>1</v>
@@ -1846,10 +2056,10 @@
         <v>136</v>
       </c>
       <c r="T11" s="4" t="n">
-        <v>350.0</v>
+        <v>275.0</v>
       </c>
       <c r="U11" s="4" t="n">
-        <v>350.0</v>
+        <v>275.0</v>
       </c>
       <c r="V11" s="3" t="n">
         <v>1</v>
@@ -1893,7 +2103,7 @@
         <v>142</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="L12" s="0" t="s">
         <v>35</v>
@@ -1965,7 +2175,7 @@
         <v>152</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="L13" s="0" t="s">
         <v>35</v>
@@ -2037,7 +2247,7 @@
         <v>162</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="L14" s="0" t="s">
         <v>35</v>
@@ -2062,10 +2272,10 @@
         <v>167</v>
       </c>
       <c r="T14" s="4" t="n">
-        <v>210.0</v>
+        <v>220.0</v>
       </c>
       <c r="U14" s="4" t="n">
-        <v>210.0</v>
+        <v>220.0</v>
       </c>
       <c r="V14" s="3" t="n">
         <v>1</v>
@@ -2109,7 +2319,7 @@
         <v>173</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="L15" s="0" t="s">
         <v>35</v>
@@ -2134,10 +2344,10 @@
         <v>178</v>
       </c>
       <c r="T15" s="4" t="n">
-        <v>220.0</v>
+        <v>210.0</v>
       </c>
       <c r="U15" s="4" t="n">
-        <v>220.0</v>
+        <v>210.0</v>
       </c>
       <c r="V15" s="3" t="n">
         <v>1</v>
@@ -2356,13 +2566,13 @@
         <v>245.0</v>
       </c>
       <c r="V18" s="3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W18" s="3" t="n">
         <v>0</v>
       </c>
       <c r="X18" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -2428,13 +2638,13 @@
         <v>245.0</v>
       </c>
       <c r="V19" s="3" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W19" s="3" t="n">
         <v>0</v>
       </c>
       <c r="X19" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20">
@@ -2494,10 +2704,10 @@
         <v>234</v>
       </c>
       <c r="T20" s="4" t="n">
-        <v>210.0</v>
+        <v>245.0</v>
       </c>
       <c r="U20" s="4" t="n">
-        <v>210.0</v>
+        <v>245.0</v>
       </c>
       <c r="V20" s="3" t="n">
         <v>1</v>
@@ -2566,10 +2776,10 @@
         <v>244</v>
       </c>
       <c r="T21" s="4" t="n">
-        <v>245.0</v>
+        <v>390.0</v>
       </c>
       <c r="U21" s="4" t="n">
-        <v>245.0</v>
+        <v>390.0</v>
       </c>
       <c r="V21" s="3" t="n">
         <v>1</v>
@@ -2638,10 +2848,10 @@
         <v>254</v>
       </c>
       <c r="T22" s="4" t="n">
-        <v>390.0</v>
+        <v>210.0</v>
       </c>
       <c r="U22" s="4" t="n">
-        <v>390.0</v>
+        <v>210.0</v>
       </c>
       <c r="V22" s="3" t="n">
         <v>1</v>
@@ -2651,6 +2861,426 @@
       </c>
       <c r="X22" s="0" t="n">
         <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="I23" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="L23" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="M23" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="N23" s="0"/>
+      <c r="O23" s="0"/>
+      <c r="P23" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="Q23" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="R23" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="S23" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="T23" s="4" t="n">
+        <v>230.0</v>
+      </c>
+      <c r="U23" s="4" t="n">
+        <v>230.0</v>
+      </c>
+      <c r="V23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W23" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X23" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="H24" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="I24" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="L24" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="M24" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="N24" s="0"/>
+      <c r="O24" s="0"/>
+      <c r="P24" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q24" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="R24" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="S24" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="T24" s="4" t="n">
+        <v>190.0</v>
+      </c>
+      <c r="U24" s="4" t="n">
+        <v>190.0</v>
+      </c>
+      <c r="V24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W24" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X24" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="F25" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>281</v>
+      </c>
+      <c r="I25" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="K25" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="L25" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="M25" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="N25" s="0"/>
+      <c r="O25" s="0"/>
+      <c r="P25" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q25" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="R25" s="0" t="s">
+        <v>286</v>
+      </c>
+      <c r="S25" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="T25" s="4" t="n">
+        <v>190.0</v>
+      </c>
+      <c r="U25" s="4" t="n">
+        <v>190.0</v>
+      </c>
+      <c r="V25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W25" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X25" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="F26" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>292</v>
+      </c>
+      <c r="I26" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="K26" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="L26" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="M26" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="N26" s="0"/>
+      <c r="O26" s="0"/>
+      <c r="P26" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="Q26" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="R26" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="S26" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="T26" s="4" t="n">
+        <v>250.0</v>
+      </c>
+      <c r="U26" s="4" t="n">
+        <v>250.0</v>
+      </c>
+      <c r="V26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X26" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>300</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="F27" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="H27" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="I27" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="K27" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="L27" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="M27" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="N27" s="0"/>
+      <c r="O27" s="0"/>
+      <c r="P27" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="Q27" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="R27" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="S27" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="T27" s="4" t="n">
+        <v>250.0</v>
+      </c>
+      <c r="U27" s="4" t="n">
+        <v>250.0</v>
+      </c>
+      <c r="V27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X27" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="s">
+        <v>308</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="F28" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="I28" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="K28" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="L28" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="M28" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="N28" s="0"/>
+      <c r="O28" s="0"/>
+      <c r="P28" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="Q28" s="0" t="s">
+        <v>316</v>
+      </c>
+      <c r="R28" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="S28" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="T28" s="4" t="n">
+        <v>250.0</v>
+      </c>
+      <c r="U28" s="4" t="n">
+        <v>250.0</v>
+      </c>
+      <c r="V28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="X28" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2689,66 +3319,66 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="9" t="s">
-        <v>255</v>
+        <v>319</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>256</v>
+        <v>320</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>257</v>
+        <v>321</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>258</v>
+        <v>322</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>259</v>
+        <v>323</v>
       </c>
       <c r="F1" s="10" t="s">
-        <v>260</v>
+        <v>324</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>261</v>
+        <v>325</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>262</v>
+        <v>326</v>
       </c>
       <c r="I1" s="9" t="s">
-        <v>263</v>
+        <v>327</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>264</v>
+        <v>328</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>265</v>
+        <v>329</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>266</v>
+        <v>330</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>267</v>
+        <v>331</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>268</v>
+        <v>332</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>269</v>
+        <v>333</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>0.145</v>
+        <v>0.147</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>270</v>
+        <v>334</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>271</v>
+        <v>335</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>272</v>
+        <v>336</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>273</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>